<commit_message>
12th Botany U_02 Q&A
</commit_message>
<xml_diff>
--- a/tamil_biology/12th_Bio_Botany_Tamil_Full.xlsx
+++ b/tamil_biology/12th_Bio_Botany_Tamil_Full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D89EB99-5B0A-42D2-9D52-C9CF80F1EBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C467A1FD-39B0-44C6-9F5C-5434B1B17697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2805,6 +2805,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1245678910" displayName="Table1245678910" ref="A1:L175" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L175" xr:uid="{138F8B09-4E29-44E2-B58F-3D298E1C4169}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="உயிரிதொழில்நுட்பவியல்"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="question_no" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="question" dataDxfId="10"/>
@@ -3201,7 +3208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3236,7 +3243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3271,7 +3278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3306,7 +3313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3341,7 +3348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3376,7 +3383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3411,7 +3418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3446,7 +3453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3481,7 +3488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3516,7 +3523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3551,7 +3558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3586,7 +3593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3621,7 +3628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3691,7 +3698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3726,7 +3733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3761,7 +3768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3796,7 +3803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3831,7 +3838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3866,7 +3873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3901,7 +3908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3936,7 +3943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3971,7 +3978,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4006,7 +4013,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4041,7 +4048,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4076,7 +4083,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4111,7 +4118,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4146,7 +4153,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -4181,7 +4188,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4217,7 +4224,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4253,7 +4260,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4288,7 +4295,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -4324,7 +4331,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -4359,7 +4366,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -4394,7 +4401,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -4429,7 +4436,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4464,7 +4471,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4499,7 +4506,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4570,7 +4577,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4605,7 +4612,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4640,7 +4647,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4675,7 +4682,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4710,7 +4717,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4745,7 +4752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4780,7 +4787,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4815,7 +4822,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4850,7 +4857,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4885,7 +4892,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4920,7 +4927,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4955,7 +4962,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4990,7 +4997,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -5025,7 +5032,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -5060,7 +5067,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -5095,7 +5102,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -5130,7 +5137,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -5144,7 +5151,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -5179,7 +5186,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -5214,7 +5221,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -5249,7 +5256,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -5284,7 +5291,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5319,7 +5326,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5354,7 +5361,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5389,7 +5396,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5424,7 +5431,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5459,7 +5466,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5494,7 +5501,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5529,7 +5536,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5543,7 +5550,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5578,7 +5585,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5613,7 +5620,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5648,7 +5655,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5683,7 +5690,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5788,7 +5795,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5823,7 +5830,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5858,7 +5865,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5998,7 +6005,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -6257,7 +6264,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -6292,7 +6299,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -6362,7 +6369,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -6397,7 +6404,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -6572,7 +6579,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -6644,7 +6651,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -6896,7 +6903,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -6932,7 +6939,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -6968,7 +6975,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -7004,7 +7011,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -7040,7 +7047,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -7076,7 +7083,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -7112,7 +7119,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -7148,7 +7155,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -7184,7 +7191,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -7220,7 +7227,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -7256,7 +7263,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -7292,7 +7299,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -7328,7 +7335,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -7364,7 +7371,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -7400,7 +7407,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -7422,7 +7429,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -7458,7 +7465,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -7494,7 +7501,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -7530,7 +7537,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -7566,7 +7573,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -7602,7 +7609,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -7638,7 +7645,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -7674,7 +7681,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -7710,7 +7717,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -7746,7 +7753,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -7782,7 +7789,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -7818,7 +7825,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -7854,7 +7861,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -7890,7 +7897,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -7912,7 +7919,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -7934,7 +7941,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -7970,7 +7977,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -7992,7 +7999,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -8028,7 +8035,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -8064,7 +8071,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -8100,7 +8107,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -8136,7 +8143,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -8172,7 +8179,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -8208,7 +8215,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -8244,7 +8251,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -8279,7 +8286,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -8314,7 +8321,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -8349,7 +8356,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -8384,7 +8391,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -8419,7 +8426,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -8454,7 +8461,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -8489,7 +8496,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -8524,7 +8531,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -8559,7 +8566,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -8594,7 +8601,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -8629,7 +8636,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -8664,7 +8671,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -8699,7 +8706,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -8734,7 +8741,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -8769,7 +8776,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -8804,7 +8811,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -8839,7 +8846,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -8874,7 +8881,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -8909,7 +8916,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -8944,7 +8951,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -8979,7 +8986,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -9014,7 +9021,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -9049,7 +9056,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -9084,7 +9091,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -9119,7 +9126,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -9154,7 +9161,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -9189,7 +9196,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>174</v>
       </c>

</xml_diff>